<commit_message>
Chatgtp Detail Added in Excel FIle
</commit_message>
<xml_diff>
--- a/Jenkin_WA.xlsx
+++ b/Jenkin_WA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pradeep\Spectrum Analyzer\Jenk_Jira_Git_Org\Jenkin\JenkinStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCD1637-D3A1-4E9F-8B93-0688900A2722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5622278E-F220-4ABB-B6E3-20636F169218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2565" windowWidth="25785" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JenkinLoginDetails" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Password</t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>update2</t>
+  </si>
+  <si>
+    <t>Chatgpt</t>
+  </si>
+  <si>
+    <t>Q1w2e3PKS$</t>
+  </si>
+  <si>
+    <t>Pradeep Singh</t>
+  </si>
+  <si>
+    <t>sk-proj-IIKi0IedwDaawn9g0ub6T3BlbkFJSh9D0PLxso1MJC6Zjll9</t>
+  </si>
+  <si>
+    <t>OpenAI</t>
+  </si>
+  <si>
+    <t>https://openai.com/</t>
   </si>
 </sst>
 </file>
@@ -427,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +552,42 @@
         <v>22</v>
       </c>
     </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EDC77441-181E-4FC2-9189-7AEC62A942F4}"/>
@@ -541,6 +595,8 @@
     <hyperlink ref="C14" r:id="rId3" xr:uid="{6C324135-758B-4825-B635-9F6612CE19F6}"/>
     <hyperlink ref="C15" r:id="rId4" xr:uid="{7A8752A7-CB71-41C1-89D9-394D71AC08CC}"/>
     <hyperlink ref="C17" r:id="rId5" xr:uid="{C57B0824-59C0-4191-8E68-2994F51C69D6}"/>
+    <hyperlink ref="C23" r:id="rId6" xr:uid="{C50EFB8D-F115-4DFC-8F42-88CEDD7670EA}"/>
+    <hyperlink ref="C27" r:id="rId7" xr:uid="{D884D781-473F-4DEE-A458-AF88D42712B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel File Reset to defeault
</commit_message>
<xml_diff>
--- a/Jenkin_WA.xlsx
+++ b/Jenkin_WA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pradeep\Spectrum Analyzer\Jenk_Jira_Git_Org\Jenkin\JenkinStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD7B4FD-59CB-4D0B-8C4B-B3A8AE7BD9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B191351-E7ED-4346-85E3-F942764A1B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Password</t>
   </si>
@@ -130,18 +130,6 @@
   </si>
   <si>
     <t>Jenkins BuildTag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git tag </t>
-  </si>
-  <si>
-    <t>v.1.1</t>
-  </si>
-  <si>
-    <t>v.1.2</t>
-  </si>
-  <si>
-    <t>v.1.3</t>
   </si>
 </sst>
 </file>
@@ -662,39 +650,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CD8DBA-403B-484E-85CC-A3BAA805C26A}">
-  <dimension ref="B2:C6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E14" sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>